<commit_message>
Updated assets to cover production usecase
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LB10019\Documents\UiPath\Välfärd\ValfardNyanställdUtbildningsKontroll\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7214869-99E8-4DF5-8AA9-E2F195D6B886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC58CA3-49A1-45DF-9A4C-39648DA97FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22485" yWindow="2805" windowWidth="28800" windowHeight="15315" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -153,46 +153,58 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
+    <t>OepCallbackUrl</t>
+  </si>
+  <si>
+    <t>OepCaseAdmID</t>
+  </si>
+  <si>
+    <t>OepDomainUrl</t>
+  </si>
+  <si>
+    <t>OepEndStatus</t>
+  </si>
+  <si>
+    <t>OepFailedStatus</t>
+  </si>
+  <si>
+    <t>OepStartStatus</t>
+  </si>
+  <si>
+    <t>ValfardNyanställdUtbildningsKontroll</t>
+  </si>
+  <si>
+    <t>Oep_Ärenden_UtbildningskontrollVälfärd</t>
+  </si>
+  <si>
+    <t>TempFolder</t>
+  </si>
+  <si>
+    <t>Grade_ExpectedUser</t>
+  </si>
+  <si>
+    <t>Grade_Credential</t>
+  </si>
+  <si>
+    <t>OepFamilyID</t>
+  </si>
+  <si>
+    <t>OepBusinessRuleStatus</t>
+  </si>
+  <si>
+    <t>OepCallbackUrl_Internal</t>
+  </si>
+  <si>
+    <t>OepDomainUrl_Internal</t>
+  </si>
+  <si>
+    <t>OepCredentials_Internal</t>
+  </si>
+  <si>
+    <t>OepCaseAdmID_Internal</t>
+  </si>
+  <si>
     <t>OepCredentials</t>
-  </si>
-  <si>
-    <t>OepCallbackUrl</t>
-  </si>
-  <si>
-    <t>OepCaseAdmID</t>
-  </si>
-  <si>
-    <t>OepDomainUrl</t>
-  </si>
-  <si>
-    <t>OepEndStatus</t>
-  </si>
-  <si>
-    <t>OepFailedStatus</t>
-  </si>
-  <si>
-    <t>OepStartStatus</t>
-  </si>
-  <si>
-    <t>ValfardNyanställdUtbildningsKontroll</t>
-  </si>
-  <si>
-    <t>Oep_Ärenden_UtbildningskontrollVälfärd</t>
-  </si>
-  <si>
-    <t>TempFolder</t>
-  </si>
-  <si>
-    <t>Grade_ExpectedUser</t>
-  </si>
-  <si>
-    <t>Grade_Credential</t>
-  </si>
-  <si>
-    <t>OepFamilyID</t>
-  </si>
-  <si>
-    <t>OepBusinessRuleStatus</t>
   </si>
 </sst>
 </file>
@@ -582,12 +594,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.54296875" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -629,13 +641,13 @@
         <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -645,12 +657,12 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
@@ -1660,16 +1672,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.54296875" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1706,7 +1718,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1717,7 +1729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1825,7 +1837,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1838,18 +1850,18 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2831,16 +2843,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.453125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2889,82 +2901,82 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>